<commit_message>
Mise à jour du fonds des générations
</commit_message>
<xml_diff>
--- a/simfin/genfund/historical_accounts.xlsx
+++ b/simfin/genfund/historical_accounts.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francois\git\simfin\simfin\genfund\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD37BDC-1300-4E57-9582-A5138492935F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2C5F4D-A193-4DBA-B250-487996FE07E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="1065" windowWidth="28005" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>account</t>
   </si>
@@ -63,6 +64,9 @@
   </si>
   <si>
     <t>hydro_indexation</t>
+  </si>
+  <si>
+    <t>placements</t>
   </si>
 </sst>
 </file>
@@ -462,7 +466,7 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -898,21 +902,63 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>36</v>
+      </c>
+      <c r="G7" s="2">
+        <v>-50</v>
+      </c>
+      <c r="H7" s="2">
+        <v>60</v>
+      </c>
+      <c r="I7" s="2">
+        <v>94</v>
+      </c>
+      <c r="J7" s="2">
+        <v>149</v>
+      </c>
+      <c r="K7" s="2">
+        <v>232</v>
+      </c>
+      <c r="L7" s="2">
+        <v>339</v>
+      </c>
+      <c r="M7" s="2">
+        <v>315</v>
+      </c>
+      <c r="N7" s="2">
+        <v>298</v>
+      </c>
+      <c r="O7" s="2">
+        <v>422</v>
+      </c>
+      <c r="P7" s="2">
+        <v>412</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1394</v>
+      </c>
+      <c r="R7" s="2">
+        <v>464</v>
+      </c>
+      <c r="S7" s="2">
+        <v>769</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changement rendement fdg valeur compatble
- La valeur comptable est obtenu avec des coeff. de reg. linéaire.
- On utilise deux lag de la valeur de marché
</commit_message>
<xml_diff>
--- a/simfin/genfund/historical_accounts.xlsx
+++ b/simfin/genfund/historical_accounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francois\git\simfin\simfin\genfund\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007BD2BA-CECD-4A50-BEE5-29EAF9667850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92030738-E24F-47C3-82F2-C366458BDE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38865" yWindow="2235" windowWidth="37335" windowHeight="18345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39165" yWindow="1785" windowWidth="33870" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>account</t>
   </si>
@@ -72,12 +72,21 @@
   </si>
   <si>
     <t>book_value</t>
+  </si>
+  <si>
+    <t>book_value_return</t>
+  </si>
+  <si>
+    <t>market_value_return</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -136,7 +145,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -163,6 +172,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,10 +490,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1095,6 +1105,124 @@
         <v>16049</v>
       </c>
     </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="14">
+        <v>1.0273972602739725E-2</v>
+      </c>
+      <c r="F10" s="14">
+        <v>3.962575674188222E-2</v>
+      </c>
+      <c r="G10" s="14">
+        <v>-3.1397174254317109E-2</v>
+      </c>
+      <c r="H10" s="14">
+        <v>2.592352559948153E-2</v>
+      </c>
+      <c r="I10" s="14">
+        <v>3.0749100425253518E-2</v>
+      </c>
+      <c r="J10" s="14">
+        <v>3.8631060409644799E-2</v>
+      </c>
+      <c r="K10" s="14">
+        <v>4.8765107724645297E-2</v>
+      </c>
+      <c r="L10" s="14">
+        <v>6.2218959346609155E-2</v>
+      </c>
+      <c r="M10" s="14">
+        <v>5.0011907597046913E-2</v>
+      </c>
+      <c r="N10" s="14">
+        <v>3.855109961190168E-2</v>
+      </c>
+      <c r="O10" s="14">
+        <v>4.431609346285114E-2</v>
+      </c>
+      <c r="P10" s="14">
+        <v>3.5305711470071555E-2</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>0.13207636553128996</v>
+      </c>
+      <c r="R10" s="14">
+        <v>5.397859469520707E-2</v>
+      </c>
+      <c r="S10" s="14">
+        <v>7.2853015015868508E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="F11" s="14">
+        <v>-0.224</v>
+      </c>
+      <c r="G11" s="14">
+        <v>0.113</v>
+      </c>
+      <c r="H11" s="14">
+        <v>0.123</v>
+      </c>
+      <c r="I11" s="14">
+        <v>0.04</v>
+      </c>
+      <c r="J11" s="14">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="K11" s="14">
+        <v>0.12</v>
+      </c>
+      <c r="L11" s="14">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="M11" s="14">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="N11" s="14">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="O11" s="14">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="P11" s="14">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="Q11" s="14">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="R11" s="14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S11" s="14">
+        <v>0.114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add elasticity and shock to FDG
- and fix futur value
</commit_message>
<xml_diff>
--- a/simfin/genfund/historical_accounts.xlsx
+++ b/simfin/genfund/historical_accounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francois\git\simfin\simfin\genfund\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92030738-E24F-47C3-82F2-C366458BDE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F371E0-F7FA-45B4-B616-6B344D2FB61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39165" yWindow="1785" windowWidth="33870" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>account</t>
   </si>
@@ -493,7 +493,7 @@
   <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -584,8 +584,8 @@
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+      <c r="B2" s="1">
+        <v>0</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -659,7 +659,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -725,7 +725,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -798,11 +798,11 @@
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>3</v>
+      <c r="B5" s="4">
+        <v>1</v>
       </c>
       <c r="C5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>

</xml_diff>